<commit_message>
Improved iron trapdoor texture
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PrismLauncher\instances\NeoBeta Remastered\minecraft\resourcepacks\Classic-Reimagined-RT3s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A201EA09-3FB9-4D7E-9319-4196148A026C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A25BCC-EE6B-4261-A1D3-1B94E02ADEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Changed nylium textures</t>
+  </si>
+  <si>
+    <t>Fixed lightmap in the nether(1.21.6)</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5"/>
@@ -594,6 +597,9 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>

</xml_diff>

<commit_message>
added textures for 26.1
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PrismLauncher\instances\NeoBeta Remastered\minecraft\resourcepacks\Classic-Reimagined-RT3s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E911A6-B375-4BAA-9D73-9F6EED2B12B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9409B983-5CAC-4B5B-9118-3B1BA9A4688B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -648,6 +648,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="21" ht="16.5" customHeight="1"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A29">

</xml_diff>

<commit_message>
Update changelog.xlsx with latest changes
The changelog spreadsheet has been updated to reflect recent modifications. Review the file for details on the latest changes.
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PrismLauncher\instances\NeoBeta Remastered\minecraft\resourcepacks\Classic-Reimagined-RT3s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF603D09-ACB4-4BAD-9181-DC02A8007E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC4A030-DEF8-4EAA-ABBA-90E7F7802B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="421" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Current version changelog" sheetId="1" r:id="rId1"/>
+    <sheet name="Active releases" sheetId="2" r:id="rId2"/>
+    <sheet name="Deprecated releases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="77">
   <si>
     <t>Minecraft Version</t>
   </si>
@@ -113,20 +115,167 @@
     <t>Changed infested cobblestone texture</t>
   </si>
   <si>
-    <t>Classic_Reimagined_10_SE_2.1</t>
-  </si>
-  <si>
     <t>Resource Name</t>
   </si>
   <si>
     <t>Resource Pack Release</t>
+  </si>
+  <si>
+    <t>1.21.11</t>
+  </si>
+  <si>
+    <t>1.21.9</t>
+  </si>
+  <si>
+    <t>1.21.6</t>
+  </si>
+  <si>
+    <t>1.21.5</t>
+  </si>
+  <si>
+    <t>v10.0.11</t>
+  </si>
+  <si>
+    <t>v10.0</t>
+  </si>
+  <si>
+    <t>1.21.4</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Classic_Reimagined_10s</t>
+  </si>
+  <si>
+    <t>1.21.2</t>
+  </si>
+  <si>
+    <t>1.20.5 / 1.21</t>
+  </si>
+  <si>
+    <t>Classic_Reimagined_10</t>
+  </si>
+  <si>
+    <t>Classic Reimagined 10 version history</t>
+  </si>
+  <si>
+    <t>_SE_2.1</t>
+  </si>
+  <si>
+    <t>_SE_2</t>
+  </si>
+  <si>
+    <t>Core version</t>
+  </si>
+  <si>
+    <t>_SE</t>
+  </si>
+  <si>
+    <t>First Release</t>
+  </si>
+  <si>
+    <t>Classic Reimagined 8 version history</t>
+  </si>
+  <si>
+    <t>Second Release</t>
+  </si>
+  <si>
+    <t>v8.10</t>
+  </si>
+  <si>
+    <t>Classic_Reimagined_8</t>
+  </si>
+  <si>
+    <t>1.20.3</t>
+  </si>
+  <si>
+    <t>1.20.2</t>
+  </si>
+  <si>
+    <t>v7.11</t>
+  </si>
+  <si>
+    <t>Better_Default_7</t>
+  </si>
+  <si>
+    <t>Better Default 7 version history</t>
+  </si>
+  <si>
+    <t>1.20 / 1.20.1</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>Better_Default_6</t>
+  </si>
+  <si>
+    <t>1.19.x</t>
+  </si>
+  <si>
+    <t>1.18.x</t>
+  </si>
+  <si>
+    <t>Better_Default_5</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>1.17.x</t>
+  </si>
+  <si>
+    <t>Better_Default_4</t>
+  </si>
+  <si>
+    <t>Better_Default_3</t>
+  </si>
+  <si>
+    <t>Better_Default_2</t>
+  </si>
+  <si>
+    <t>Patch</t>
+  </si>
+  <si>
+    <t>Minor version</t>
+  </si>
+  <si>
+    <t>Better_Default</t>
+  </si>
+  <si>
+    <t>1.16.2</t>
+  </si>
+  <si>
+    <t>Better Default Legacy version history</t>
+  </si>
+  <si>
+    <t>Better Default 6</t>
+  </si>
+  <si>
+    <t>Better Default 5</t>
+  </si>
+  <si>
+    <t>Better Default 4</t>
+  </si>
+  <si>
+    <t>Better Default 3</t>
+  </si>
+  <si>
+    <t>Better Default 2</t>
+  </si>
+  <si>
+    <t>Better Default 1.1</t>
+  </si>
+  <si>
+    <t>Better Default 1.1a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +312,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +355,18 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0078D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD75B00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -263,19 +431,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -287,6 +455,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -305,17 +474,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,6 +573,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFD75B00"/>
+      <color rgb="FF0078D7"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -580,18 +768,18 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.25" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -607,15 +795,15 @@
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -626,161 +814,1380 @@
         <f>SUM(2601,637,2026,27,41)</f>
         <v>5332</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>26.1</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="13" t="str">
-        <f>A2 &amp; "_" &amp; B2 &amp; "-" &amp; B3</f>
-        <v>10.0.11_1-Classic_Reimagined_10_SE_2.1</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="13" t="str">
-        <f>B4 &amp; "-build-" &amp; C2</f>
-        <v>10.0.11_1-Classic_Reimagined_10_SE_2.1-build-5332</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="E5" s="3"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="16.5" customHeight="1"/>
+    <row r="21" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:A17">
-    <sortCondition ref="A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A14">
+    <sortCondition ref="A14"/>
   </sortState>
   <mergeCells count="3">
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="F2:J2"/>
+    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A590D7F-A585-4A26-BECF-864B2B6E4598}">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <f>SUM(2601,637,2026,27,41)</f>
+        <v>5332</v>
+      </c>
+      <c r="D4" s="6">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16" t="str">
+        <f xml:space="preserve"> "Classic_Reimagined_10" &amp; A2</f>
+        <v>Classic_Reimagined_10_SE_2.1</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="16" t="str">
+        <f>A4 &amp; "_" &amp; B4 &amp; "-" &amp; B5</f>
+        <v>v10.0.11_1-Classic_Reimagined_10_SE_2.1</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="16" t="str">
+        <f>B6 &amp; "-build-" &amp; C4</f>
+        <v>v10.0.11_1-Classic_Reimagined_10_SE_2.1-build-5332</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6">
+        <f>C4</f>
+        <v>5332</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="16" t="str">
+        <f xml:space="preserve"> "Classic_Reimagined_10" &amp; A8</f>
+        <v>Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="16" t="str">
+        <f>A10 &amp; "." &amp; B10 &amp; "-" &amp; B11</f>
+        <v>v10.0.10-Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="16" t="str">
+        <f>B12 &amp; "-build-" &amp; C10</f>
+        <v>v10.0.10-Classic_Reimagined_10_SE_2-build-5332</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6">
+        <f>C10</f>
+        <v>5332</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="16" t="str">
+        <f xml:space="preserve"> B11</f>
+        <v>Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="16" t="str">
+        <f>A15 &amp; "." &amp; B15 &amp; "-" &amp; B16</f>
+        <v>v10.0.9-Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="16" t="str">
+        <f>B17 &amp; "-build-" &amp; C15</f>
+        <v>v10.0.9-Classic_Reimagined_10_SE_2-build-5332</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6">
+        <f>C15</f>
+        <v>5332</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="16" t="str">
+        <f xml:space="preserve"> B16</f>
+        <v>Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="16" t="str">
+        <f>A20 &amp; "." &amp; B20 &amp; "-" &amp; B21</f>
+        <v>v10.0.7-Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="16" t="str">
+        <f>B22 &amp; "-build-" &amp; C20</f>
+        <v>v10.0.7-Classic_Reimagined_10_SE_2-build-5332</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="6">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6">
+        <f>C20</f>
+        <v>5332</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="str">
+        <f xml:space="preserve"> B21</f>
+        <v>Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="str">
+        <f>A25 &amp; "." &amp; B25 &amp; "-" &amp; B26</f>
+        <v>v10.0.4-Classic_Reimagined_10_SE_2</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="16" t="str">
+        <f>B27 &amp; "-build-" &amp; C25</f>
+        <v>v10.0.4-Classic_Reimagined_10_SE_2-build-5332</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="6">
+        <v>3</v>
+      </c>
+      <c r="C31" s="6">
+        <f>C25</f>
+        <v>5332</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="16" t="str">
+        <f xml:space="preserve"> "Classic_Reimagined_10" &amp; A29</f>
+        <v>Classic_Reimagined_10_SE</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="16" t="str">
+        <f>A31 &amp; "." &amp; B31 &amp; "-" &amp; B32</f>
+        <v>v10.0.3-Classic_Reimagined_10_SE</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="16" t="str">
+        <f>B33 &amp; "-build-" &amp; C31</f>
+        <v>v10.0.3-Classic_Reimagined_10_SE-build-5332</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="6">
+        <v>2</v>
+      </c>
+      <c r="C37" s="6">
+        <f>C31</f>
+        <v>5332</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="16" t="str">
+        <f>A37 &amp; "." &amp; B37 &amp; "-" &amp; B38</f>
+        <v>v10.0.2-Classic_Reimagined_10s</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="16" t="str">
+        <f>B39 &amp; "-build-" &amp; C37</f>
+        <v>v10.0.2-Classic_Reimagined_10s-build-5332</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6">
+        <f>C37</f>
+        <v>5332</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="16" t="str">
+        <f>A43 &amp; "." &amp; B43 &amp; "-" &amp; B44</f>
+        <v>v10.0.1-Classic_Reimagined_10</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="16" t="str">
+        <f>B45 &amp; "-build-" &amp; C43</f>
+        <v>v10.0.1-Classic_Reimagined_10-build-5332</v>
+      </c>
+      <c r="C46" s="17"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="6">
+        <v>32</v>
+      </c>
+      <c r="C50" s="6">
+        <f>C43</f>
+        <v>5332</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="16" t="str">
+        <f>A50 &amp; "." &amp; B50 &amp; "-" &amp; B51</f>
+        <v>v8.10.32-Classic_Reimagined_8</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="16" t="str">
+        <f>B52 &amp; "-build-" &amp; C50</f>
+        <v>v8.10.32-Classic_Reimagined_8-build-5332</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="6">
+        <v>31</v>
+      </c>
+      <c r="C56" s="6">
+        <f>C50</f>
+        <v>5332</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="16" t="str">
+        <f>A56 &amp; "." &amp; B56 &amp; "-" &amp; B57</f>
+        <v>v8.10.31-Classic_Reimagined_8</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="16" t="str">
+        <f>B58 &amp; "-build-" &amp; C56</f>
+        <v>v8.10.31-Classic_Reimagined_8-build-5332</v>
+      </c>
+      <c r="C59" s="17"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+    </row>
+    <row r="61" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="6">
+        <v>3</v>
+      </c>
+      <c r="C62" s="6">
+        <f>C56</f>
+        <v>5332</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="16" t="str">
+        <f>A62 &amp; "." &amp; B62 &amp; "-" &amp; B63</f>
+        <v>v7.11.3-Better_Default_7</v>
+      </c>
+      <c r="C64" s="17"/>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="16" t="str">
+        <f>B64 &amp; "-build-" &amp; C62</f>
+        <v>v7.11.3-Better_Default_7-build-5332</v>
+      </c>
+      <c r="C65" s="17"/>
+      <c r="D65" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F5664-A36C-46AF-906D-AC064FC4072D}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="22">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>A4 &amp; "." &amp; B4 &amp; "." &amp; C4 &amp; "-" &amp; B5</f>
+        <v>v6.0.7-Better_Default_6</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="22">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>A9 &amp; "." &amp; B9 &amp; "." &amp; C9 &amp; "-" &amp; B10</f>
+        <v>v1.4.0-Better_Default_5</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="22">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>A14 &amp; "." &amp; B14 &amp; "." &amp; C14 &amp; "-" &amp; B15</f>
+        <v>v1.3.0-Better_Default_4</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="22">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="18" t="str">
+        <f>A19 &amp; "." &amp; B19 &amp; "." &amp; C19 &amp; "-" &amp; B20</f>
+        <v>v1.2.2-Better_Default_3</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="22">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="18" t="str">
+        <f>A24 &amp; "." &amp; B24 &amp; "." &amp; C24 &amp; "-" &amp; B25</f>
+        <v>v1.2.1-Better_Default_3</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="22">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="18" t="str">
+        <f>A29 &amp; "." &amp; B29 &amp; "." &amp; C29 &amp; "-" &amp; B30</f>
+        <v>v1.2.0-Better_Default_2</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="22">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="18" t="str">
+        <f>A34 &amp; "." &amp; B34 &amp; "." &amp; C34 &amp; "-" &amp; B35</f>
+        <v>v1.1.1-Better_Default</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="22">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="18" t="str">
+        <f>A39 &amp; "." &amp; B39 &amp; "." &amp; C39 &amp; "-" &amp; B40</f>
+        <v>v1.1.0-Better_Default</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>